<commit_message>
Casos de uso :100:
</commit_message>
<xml_diff>
--- a/Tabla Pivote.xlsx
+++ b/Tabla Pivote.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="106">
   <si>
     <t>Proyecto #1 Bases de Datos</t>
   </si>
@@ -330,6 +330,18 @@
   </si>
   <si>
     <t>Despliega el catálogo de Dsitritos cuando se filtra</t>
+  </si>
+  <si>
+    <t>No permite 2 correos iguales</t>
+  </si>
+  <si>
+    <t>El sistema no permite que hayan dos correos iguales</t>
+  </si>
+  <si>
+    <t>Reporte de cumpleaños</t>
+  </si>
+  <si>
+    <t>General un reporte el día del cumpleaños del usuario</t>
   </si>
 </sst>
 </file>
@@ -414,12 +426,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -428,6 +434,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,17 +828,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D12047-B004-4F53-91F8-3D54840BC53B}">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="6" customWidth="1"/>
     <col min="4" max="4" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="68" style="4" customWidth="1"/>
     <col min="6" max="6" width="39.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="4" customWidth="1"/>
     <col min="8" max="11" width="11.42578125" style="3"/>
@@ -836,11 +848,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -857,11 +869,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="1">
@@ -876,11 +888,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="1">
@@ -895,11 +907,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="1">
@@ -914,11 +926,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="1">
@@ -933,14 +945,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
-        <v>56</v>
+      <c r="C6" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
@@ -948,14 +960,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C7" s="8" t="s">
-        <v>17</v>
+      <c r="C7" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
@@ -963,14 +975,14 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C8" s="8" t="s">
-        <v>24</v>
+      <c r="C8" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="D8" s="1">
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
@@ -978,14 +990,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C9" s="8" t="s">
-        <v>36</v>
+      <c r="C9" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
@@ -993,14 +1005,14 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C10" s="8" t="s">
-        <v>13</v>
+      <c r="C10" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="D10" s="1">
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
@@ -1008,14 +1020,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C11" s="8" t="s">
-        <v>57</v>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="1">
         <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
@@ -1023,14 +1035,14 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
-        <v>58</v>
+      <c r="C12" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="D12" s="1">
         <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
@@ -1038,14 +1050,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C13" s="8" t="s">
-        <v>59</v>
+      <c r="C13" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="D13" s="1">
         <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
@@ -1053,14 +1065,14 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C14" s="8" t="s">
-        <v>60</v>
+      <c r="C14" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="D14" s="1">
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
@@ -1068,14 +1080,14 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C15" s="8" t="s">
-        <v>61</v>
+      <c r="C15" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D15" s="1">
         <v>14</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
@@ -1083,14 +1095,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C16" s="8" t="s">
-        <v>74</v>
+      <c r="C16" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D16" s="1">
         <v>16</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
@@ -1098,14 +1110,14 @@
       </c>
     </row>
     <row r="17" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C17" s="8" t="s">
-        <v>75</v>
+      <c r="C17" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="1">
         <v>17</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
@@ -1113,14 +1125,14 @@
       </c>
     </row>
     <row r="18" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C18" s="8" t="s">
-        <v>76</v>
+      <c r="C18" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="D18" s="1">
         <v>18</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
@@ -1128,14 +1140,14 @@
       </c>
     </row>
     <row r="19" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C19" s="8" t="s">
-        <v>14</v>
+      <c r="C19" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="D19" s="1">
         <v>20</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
@@ -1143,14 +1155,14 @@
       </c>
     </row>
     <row r="20" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C20" s="8" t="s">
-        <v>72</v>
+      <c r="C20" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D20" s="1">
         <v>21</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
@@ -1158,14 +1170,14 @@
       </c>
     </row>
     <row r="21" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C21" s="8" t="s">
-        <v>19</v>
+      <c r="C21" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="D21" s="1">
         <v>22</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
@@ -1173,14 +1185,14 @@
       </c>
     </row>
     <row r="22" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C22" s="8" t="s">
-        <v>21</v>
+      <c r="C22" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="D22" s="1">
         <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
@@ -1188,14 +1200,14 @@
       </c>
     </row>
     <row r="23" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C23" s="8" t="s">
-        <v>22</v>
+      <c r="C23" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="D23" s="1">
         <v>24</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
@@ -1203,14 +1215,14 @@
       </c>
     </row>
     <row r="24" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C24" s="8" t="s">
-        <v>23</v>
+      <c r="C24" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D24" s="1">
         <v>25</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
@@ -1218,14 +1230,14 @@
       </c>
     </row>
     <row r="25" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C25" s="8" t="s">
-        <v>27</v>
+      <c r="C25" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D25" s="1">
         <v>26</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
@@ -1233,14 +1245,14 @@
       </c>
     </row>
     <row r="26" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C26" s="8" t="s">
-        <v>28</v>
+      <c r="C26" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D26" s="1">
         <v>27</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
@@ -1248,14 +1260,14 @@
       </c>
     </row>
     <row r="27" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C27" s="8" t="s">
-        <v>29</v>
+      <c r="C27" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D27" s="1">
         <v>28</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
@@ -1263,14 +1275,14 @@
       </c>
     </row>
     <row r="28" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C28" s="8" t="s">
-        <v>30</v>
+      <c r="C28" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D28" s="1">
         <v>29</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
@@ -1278,14 +1290,14 @@
       </c>
     </row>
     <row r="29" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C29" s="8" t="s">
-        <v>31</v>
+      <c r="C29" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D29" s="1">
         <v>30</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
@@ -1293,14 +1305,14 @@
       </c>
     </row>
     <row r="30" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C30" s="8" t="s">
-        <v>26</v>
+      <c r="C30" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D30" s="1">
         <v>31</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
@@ -1308,14 +1320,14 @@
       </c>
     </row>
     <row r="31" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C31" s="8" t="s">
-        <v>32</v>
+      <c r="C31" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D31" s="1">
         <v>32</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
@@ -1323,14 +1335,14 @@
       </c>
     </row>
     <row r="32" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C32" s="8" t="s">
-        <v>33</v>
+      <c r="C32" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D32" s="1">
         <v>33</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
@@ -1338,14 +1350,14 @@
       </c>
     </row>
     <row r="33" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C33" s="8" t="s">
-        <v>34</v>
+      <c r="C33" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D33" s="1">
         <v>35</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
@@ -1353,14 +1365,14 @@
       </c>
     </row>
     <row r="34" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C34" s="8" t="s">
-        <v>35</v>
+      <c r="C34" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D34" s="1">
         <v>36</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
@@ -1368,14 +1380,14 @@
       </c>
     </row>
     <row r="35" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C35" s="8" t="s">
-        <v>37</v>
+      <c r="C35" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D35" s="1">
         <v>37</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
@@ -1383,14 +1395,14 @@
       </c>
     </row>
     <row r="36" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C36" s="8" t="s">
-        <v>80</v>
+      <c r="C36" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="D36" s="1">
         <v>38</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2" t="s">
@@ -1398,14 +1410,14 @@
       </c>
     </row>
     <row r="37" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C37" s="8" t="s">
-        <v>81</v>
+      <c r="C37" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="D37" s="1">
         <v>39</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
@@ -1413,14 +1425,14 @@
       </c>
     </row>
     <row r="38" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C38" s="8" t="s">
-        <v>82</v>
+      <c r="C38" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="D38" s="1">
         <v>40</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
@@ -1428,14 +1440,14 @@
       </c>
     </row>
     <row r="39" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C39" s="8" t="s">
-        <v>83</v>
+      <c r="C39" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="D39" s="1">
         <v>41</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
@@ -1443,14 +1455,14 @@
       </c>
     </row>
     <row r="40" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C40" s="8" t="s">
-        <v>84</v>
+      <c r="C40" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="D40" s="1">
         <v>42</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
@@ -1458,14 +1470,14 @@
       </c>
     </row>
     <row r="41" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C41" s="8" t="s">
-        <v>85</v>
+      <c r="C41" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D41" s="1">
         <v>43</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
@@ -1473,14 +1485,14 @@
       </c>
     </row>
     <row r="42" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C42" s="8" t="s">
-        <v>86</v>
+      <c r="C42" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="D42" s="1">
         <v>44</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
@@ -1488,14 +1500,14 @@
       </c>
     </row>
     <row r="43" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C43" s="8" t="s">
-        <v>87</v>
+      <c r="C43" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D43" s="1">
         <v>45</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2" t="s">
@@ -1503,14 +1515,14 @@
       </c>
     </row>
     <row r="44" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C44" s="8" t="s">
-        <v>88</v>
+      <c r="C44" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D44" s="1">
         <v>46</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
@@ -1518,29 +1530,29 @@
       </c>
     </row>
     <row r="45" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C45" s="8" t="s">
-        <v>89</v>
+      <c r="C45" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D45" s="1">
         <v>47</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="10"/>
+        <v>99</v>
+      </c>
+      <c r="F45" s="8"/>
       <c r="G45" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C46" s="8" t="s">
-        <v>90</v>
+      <c r="C46" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D46" s="1">
         <v>48</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
@@ -1548,17 +1560,29 @@
       </c>
     </row>
     <row r="47" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C47" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="D47" s="1">
         <v>49</v>
       </c>
+      <c r="E47" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="3:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C48" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="D48" s="1">
         <v>50</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
@@ -1576,7 +1600,7 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
   </mergeCells>
-  <conditionalFormatting sqref="G2:G46">
+  <conditionalFormatting sqref="G2:G47">
     <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Con Error">
       <formula>NOT(ISERROR(SEARCH("Con Error",G2)))</formula>
     </cfRule>
@@ -1587,15 +1611,15 @@
       <formula>NOT(ISERROR(SEARCH("Pendiente",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47:G48">
+  <conditionalFormatting sqref="G48">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Con Error">
-      <formula>NOT(ISERROR(SEARCH("Con Error",G47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Con Error",G48)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Certificado">
-      <formula>NOT(ISERROR(SEARCH("Certificado",G47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Certificado",G48)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Pendiente">
-      <formula>NOT(ISERROR(SEARCH("Pendiente",G47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pendiente",G48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>